<commit_message>
Updated hitters and deleted hitters table
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29107"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19277BA-A8A6-4E66-9367-8A6742189E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75DA301-336B-429F-90C6-D0DCAA276A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="384" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Players!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -7009,11 +7010,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1896"/>
+  <dimension ref="A1:N1866"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1860" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1865" sqref="A1865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -87059,202 +87060,14 @@
       </c>
     </row>
     <row r="1865" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1865" t="e">
-        <f>VLOOKUP(B1865,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
       <c r="N1865" t="e">
         <f>VLOOKUP(B1865,Teams!A:C,3,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="1866" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1866" t="e">
-        <f>VLOOKUP(B1866,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
       <c r="N1866" t="e">
         <f>VLOOKUP(B1866,Teams!A:C,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1867" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1867" t="e">
-        <f>VLOOKUP(B1867,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1868" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1868" t="e">
-        <f>VLOOKUP(B1868,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1869" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1869" t="e">
-        <f>VLOOKUP(B1869,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1870" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1870" t="e">
-        <f>VLOOKUP(B1870,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1871" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1871" t="e">
-        <f>VLOOKUP(B1871,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1872" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1872" t="e">
-        <f>VLOOKUP(B1872,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1873" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1873" t="e">
-        <f>VLOOKUP(B1873,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1874" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1874" t="e">
-        <f>VLOOKUP(B1874,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1875" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1875" t="e">
-        <f>VLOOKUP(B1875,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1876" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1876" t="e">
-        <f>VLOOKUP(B1876,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1877" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1877" t="e">
-        <f>VLOOKUP(B1877,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1878" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1878" t="e">
-        <f>VLOOKUP(B1878,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1879" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1879" t="e">
-        <f>VLOOKUP(B1879,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1880" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1880" t="e">
-        <f>VLOOKUP(B1880,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1881" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1881" t="e">
-        <f>VLOOKUP(B1881,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1882" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1882" t="e">
-        <f>VLOOKUP(B1882,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1883" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1883" t="e">
-        <f>VLOOKUP(B1883,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1884" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1884" t="e">
-        <f>VLOOKUP(B1884,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1885" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1885" t="e">
-        <f>VLOOKUP(B1885,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1886" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1886" t="e">
-        <f>VLOOKUP(B1886,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1887" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1887" t="e">
-        <f>VLOOKUP(B1887,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1888" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1888" t="e">
-        <f>VLOOKUP(B1888,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1889" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1889" t="e">
-        <f>VLOOKUP(B1889,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1890" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1890" t="e">
-        <f>VLOOKUP(B1890,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1891" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1891" t="e">
-        <f>VLOOKUP(B1891,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1892" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1892" t="e">
-        <f>VLOOKUP(B1892,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1893" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1893" t="e">
-        <f>VLOOKUP(B1893,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1894" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1894" t="e">
-        <f>VLOOKUP(B1894,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1895" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1895" t="e">
-        <f>VLOOKUP(B1895,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1896" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C1896" t="e">
-        <f>VLOOKUP(B1896,Teams!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edit alter_table and hitters table
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F2EA7F-3B9A-498D-940F-E2B7CAB683F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1462DAEA-123D-481D-BB6C-D9F3E6E0AABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -7012,11 +7012,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1866"/>
+  <dimension ref="A1:N1865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1860" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1866" sqref="G1866"/>
+      <selection pane="bottomLeft" activeCell="A1863" sqref="A1863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -87076,7 +87076,7 @@
         <v>10</v>
       </c>
       <c r="E1865">
-        <v>123456</v>
+        <v>99999</v>
       </c>
       <c r="F1865" t="s">
         <v>2197</v>
@@ -87105,12 +87105,6 @@
       <c r="N1865" t="str">
         <f>VLOOKUP(B1865,Teams!A:C,3,FALSE)</f>
         <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="1866" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="N1866" t="e">
-        <f>VLOOKUP(B1866,Teams!A:C,3,FALSE)</f>
-        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update hitters one last time
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49190AFA-7685-4A91-B9CF-C221292B4B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8542703-8A25-4A10-BFA4-CCD1ADCC6CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22364" uniqueCount="2204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22365" uniqueCount="2205">
   <si>
     <t>mlb_name</t>
   </si>
@@ -6650,6 +6650,9 @@
   </si>
   <si>
     <t>Garth Brooks</t>
+  </si>
+  <si>
+    <t>Austin Powers</t>
   </si>
 </sst>
 </file>
@@ -7030,11 +7033,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1871"/>
+  <dimension ref="A1:N1872"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1860" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1871" sqref="K1871"/>
+      <selection pane="bottomLeft" activeCell="A1873" sqref="A1873"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -87244,6 +87247,14 @@
       </c>
       <c r="K1871">
         <v>123456</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1872" t="s">
+        <v>2204</v>
+      </c>
+      <c r="K1872">
+        <v>222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating hitters and workflow
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8542703-8A25-4A10-BFA4-CCD1ADCC6CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2C314F-69CB-4FEC-8D63-5E19E0BDBE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22365" uniqueCount="2205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22366" uniqueCount="2206">
   <si>
     <t>mlb_name</t>
   </si>
@@ -6653,6 +6653,9 @@
   </si>
   <si>
     <t>Austin Powers</t>
+  </si>
+  <si>
+    <t>Billy Bob Thornton</t>
   </si>
 </sst>
 </file>
@@ -7033,11 +7036,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1872"/>
+  <dimension ref="A1:N1873"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1860" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1873" sqref="A1873"/>
+      <selection pane="bottomLeft" activeCell="A1874" sqref="A1874"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -87255,6 +87258,14 @@
       </c>
       <c r="K1872">
         <v>222222</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1873" t="s">
+        <v>2205</v>
+      </c>
+      <c r="K1873">
+        <v>348242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating hitters july 13
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F526D04A-D9BB-498B-9A6B-D792007851CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFB25C3-E3B6-4D3D-9AFF-F68BEC697F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22371" uniqueCount="2211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22382" uniqueCount="2211">
   <si>
     <t>mlb_name</t>
   </si>
@@ -7053,9 +7053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1878"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1860" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1879" sqref="A1879"/>
+      <selection pane="bottomLeft" activeCell="N1879" sqref="N1879"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -87250,6 +87250,9 @@
       <c r="A1869" t="s">
         <v>2201</v>
       </c>
+      <c r="K1869">
+        <v>727272</v>
+      </c>
     </row>
     <row r="1870" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1870" t="s">
@@ -87275,7 +87278,7 @@
         <v>222222</v>
       </c>
     </row>
-    <row r="1873" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1873" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1873" t="s">
         <v>2205</v>
       </c>
@@ -87283,7 +87286,7 @@
         <v>348242</v>
       </c>
     </row>
-    <row r="1874" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1874" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1874" t="s">
         <v>2206</v>
       </c>
@@ -87291,7 +87294,7 @@
         <v>347243</v>
       </c>
     </row>
-    <row r="1875" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1875" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1875" t="s">
         <v>2207</v>
       </c>
@@ -87299,7 +87302,7 @@
         <v>843434</v>
       </c>
     </row>
-    <row r="1876" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1876" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1876" t="s">
         <v>2208</v>
       </c>
@@ -87307,7 +87310,7 @@
         <v>492887</v>
       </c>
     </row>
-    <row r="1877" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1877" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1877" t="s">
         <v>2209</v>
       </c>
@@ -87315,12 +87318,48 @@
         <v>102212</v>
       </c>
     </row>
-    <row r="1878" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1878" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1878" t="s">
         <v>2210</v>
       </c>
+      <c r="B1878" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1878" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1878" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1878">
+        <v>12345</v>
+      </c>
+      <c r="F1878" t="s">
+        <v>2210</v>
+      </c>
+      <c r="G1878" t="s">
+        <v>818</v>
+      </c>
+      <c r="H1878" t="s">
+        <v>2210</v>
+      </c>
+      <c r="I1878" t="s">
+        <v>2210</v>
+      </c>
+      <c r="J1878" t="s">
+        <v>2210</v>
+      </c>
       <c r="K1878">
         <v>112514</v>
+      </c>
+      <c r="L1878" t="s">
+        <v>2210</v>
+      </c>
+      <c r="M1878" t="s">
+        <v>2210</v>
+      </c>
+      <c r="N1878" t="s">
+        <v>2097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating hitters with test row
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C8469A-C28B-48CB-8AE3-8F374842819B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F65F68-3EE8-408C-B493-AEF95C6E4F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1620" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22361" uniqueCount="2198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22373" uniqueCount="2199">
   <si>
     <t>mlb_name</t>
   </si>
@@ -6614,6 +6614,9 @@
   </si>
   <si>
     <t>Big Pimpin</t>
+  </si>
+  <si>
+    <t>Big Daddy</t>
   </si>
 </sst>
 </file>
@@ -6981,10 +6984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1861"/>
+  <dimension ref="A1:N1862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1840" workbookViewId="0">
-      <selection activeCell="G1862" sqref="G1862"/>
+    <sheetView tabSelected="1" topLeftCell="A1842" workbookViewId="0">
+      <selection activeCell="N1862" sqref="N1862"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -84952,6 +84955,50 @@
         <v>2184</v>
       </c>
     </row>
+    <row r="1862" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1862" t="s">
+        <v>2198</v>
+      </c>
+      <c r="B1862" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C1862" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D1862" t="s">
+        <v>1934</v>
+      </c>
+      <c r="E1862">
+        <v>88888</v>
+      </c>
+      <c r="F1862" t="s">
+        <v>2198</v>
+      </c>
+      <c r="G1862" t="s">
+        <v>2074</v>
+      </c>
+      <c r="H1862" t="s">
+        <v>2198</v>
+      </c>
+      <c r="I1862" t="s">
+        <v>2198</v>
+      </c>
+      <c r="J1862" t="s">
+        <v>2198</v>
+      </c>
+      <c r="K1862">
+        <v>888888</v>
+      </c>
+      <c r="L1862" t="s">
+        <v>2198</v>
+      </c>
+      <c r="M1862" t="s">
+        <v>2198</v>
+      </c>
+      <c r="N1862" t="s">
+        <v>2198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing alter table and hitters
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F65F68-3EE8-408C-B493-AEF95C6E4F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A596CF8-BAEF-48F2-8030-9C0A2EC1D6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1620" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22373" uniqueCount="2199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22385" uniqueCount="2200">
   <si>
     <t>mlb_name</t>
   </si>
@@ -6617,6 +6617,9 @@
   </si>
   <si>
     <t>Big Daddy</t>
+  </si>
+  <si>
+    <t>Small Daddy</t>
   </si>
 </sst>
 </file>
@@ -6984,10 +6987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1862"/>
+  <dimension ref="A1:N1863"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1842" workbookViewId="0">
-      <selection activeCell="N1862" sqref="N1862"/>
+      <selection activeCell="N1863" sqref="N1863"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -84999,6 +85002,50 @@
         <v>2198</v>
       </c>
     </row>
+    <row r="1863" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1863" t="s">
+        <v>2199</v>
+      </c>
+      <c r="B1863" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C1863" t="s">
+        <v>1919</v>
+      </c>
+      <c r="D1863" t="s">
+        <v>1934</v>
+      </c>
+      <c r="E1863">
+        <v>77777</v>
+      </c>
+      <c r="F1863" t="s">
+        <v>2199</v>
+      </c>
+      <c r="G1863" t="s">
+        <v>2074</v>
+      </c>
+      <c r="H1863" t="s">
+        <v>2199</v>
+      </c>
+      <c r="I1863" t="s">
+        <v>2199</v>
+      </c>
+      <c r="J1863" t="s">
+        <v>2199</v>
+      </c>
+      <c r="K1863">
+        <v>777777</v>
+      </c>
+      <c r="L1863" t="s">
+        <v>2199</v>
+      </c>
+      <c r="M1863" t="s">
+        <v>2199</v>
+      </c>
+      <c r="N1863" t="s">
+        <v>2199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating hitters file and trying to fix the alter_table code
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D60FBBC-78C5-46A6-8748-DB57C3A9FC2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4778B6B7-C8DA-4A2E-BB96-B404477494D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="900" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2641,7 +2641,7 @@
     <t>Atlanta</t>
   </si>
   <si>
-    <t>Big D Daddy</t>
+    <t>Big Diesel</t>
   </si>
 </sst>
 </file>
@@ -3011,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A654" workbookViewId="0">
-      <selection activeCell="K656" sqref="K656"/>
+    <sheetView tabSelected="1" topLeftCell="A635" workbookViewId="0">
+      <selection activeCell="A656" sqref="A656"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Testing hitter file again
</commit_message>
<xml_diff>
--- a/api/hitters.xlsx
+++ b/api/hitters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\api\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AAA8B4-625C-42E3-853D-DD3FB29D2CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE2112E-7423-4D0B-95AD-36B9437C9A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="900" windowWidth="21600" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7922" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7934" uniqueCount="876">
   <si>
     <t>mlb_name</t>
   </si>
@@ -2645,6 +2645,9 @@
   </si>
   <si>
     <t>John Doe</t>
+  </si>
+  <si>
+    <t>Mike Jones</t>
   </si>
 </sst>
 </file>
@@ -3012,10 +3015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N660"/>
+  <dimension ref="A1:N661"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A639" workbookViewId="0">
-      <selection activeCell="G660" sqref="G660"/>
+    <sheetView tabSelected="1" topLeftCell="A640" workbookViewId="0">
+      <selection activeCell="N661" sqref="N661"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31967,6 +31970,50 @@
         <v>874</v>
       </c>
     </row>
+    <row r="661" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A661" t="s">
+        <v>875</v>
+      </c>
+      <c r="B661" t="s">
+        <v>693</v>
+      </c>
+      <c r="C661" t="s">
+        <v>723</v>
+      </c>
+      <c r="D661" t="s">
+        <v>725</v>
+      </c>
+      <c r="E661">
+        <v>83929</v>
+      </c>
+      <c r="F661" t="s">
+        <v>875</v>
+      </c>
+      <c r="G661" t="s">
+        <v>766</v>
+      </c>
+      <c r="H661" t="s">
+        <v>875</v>
+      </c>
+      <c r="I661" t="s">
+        <v>875</v>
+      </c>
+      <c r="J661" t="s">
+        <v>875</v>
+      </c>
+      <c r="K661">
+        <v>220852</v>
+      </c>
+      <c r="L661" t="s">
+        <v>875</v>
+      </c>
+      <c r="M661" t="s">
+        <v>875</v>
+      </c>
+      <c r="N661" t="s">
+        <v>875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>